<commit_message>
with viscosity curve fit
</commit_message>
<xml_diff>
--- a/AGMD_Validation_A-Khalifa-et-al_figure5.xlsx
+++ b/AGMD_Validation_A-Khalifa-et-al_figure5.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Default Dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -36,13 +37,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -79,6 +86,1073 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.787</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.519</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.307</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.798</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.653</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.547</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.467</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.404</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.355</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.315</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.282</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-971775360"/>
+        <c:axId val="-970257632"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-971775360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-970257632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-970257632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-971775360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -344,15 +1418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -372,7 +1446,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>15</v>
       </c>
@@ -391,8 +1465,11 @@
       <c r="F2">
         <v>67.808219178082197</v>
       </c>
+      <c r="H2">
+        <v>10.69</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20</v>
       </c>
@@ -412,7 +1489,7 @@
         <v>65.342465753424605</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>25</v>
       </c>
@@ -432,7 +1509,7 @@
         <v>62.4657534246575</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>30</v>
       </c>
@@ -455,4 +1532,152 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView topLeftCell="F11" zoomScale="231" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1.7869999999999999</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1.7869999999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.5189999999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.5189999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.3069999999999999</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.3069999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.002</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.80100000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.65800000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>60</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>70</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.41299999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>80</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>90</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.315</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.32600000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.29399999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>